<commit_message>
Asistencias y correciones a sistemas caóticos.
</commit_message>
<xml_diff>
--- a/Asistencias.xlsx
+++ b/Asistencias.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
   <si>
     <t>Felix Santiago Bautista</t>
   </si>
@@ -78,6 +78,15 @@
   </si>
   <si>
     <t>Isabel Valdés Ochoa</t>
+  </si>
+  <si>
+    <t>Epsilon</t>
+  </si>
+  <si>
+    <t>Esperanza</t>
+  </si>
+  <si>
+    <t>Santana</t>
   </si>
 </sst>
 </file>
@@ -401,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -430,6 +439,9 @@
       <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -438,6 +450,9 @@
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -446,6 +461,9 @@
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -454,6 +472,9 @@
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -462,6 +483,9 @@
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -470,6 +494,7 @@
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -478,6 +503,7 @@
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -486,6 +512,9 @@
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -494,6 +523,9 @@
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -502,6 +534,9 @@
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -510,30 +545,62 @@
       <c r="B12" s="2">
         <v>0.5</v>
       </c>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
+      <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
+      <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
+      <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mas ejercicios y correciones.
</commit_message>
<xml_diff>
--- a/Asistencias.xlsx
+++ b/Asistencias.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5916"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="21">
   <si>
     <t>Felix Santiago Bautista</t>
   </si>
@@ -410,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -421,7 +421,7 @@
     <col min="1" max="1" width="35.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -431,8 +431,11 @@
       <c r="C1" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -442,8 +445,11 @@
       <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -453,8 +459,11 @@
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -464,8 +473,11 @@
       <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -475,8 +487,11 @@
       <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -486,8 +501,11 @@
       <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -495,8 +513,9 @@
         <v>10</v>
       </c>
       <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -504,8 +523,9 @@
         <v>10</v>
       </c>
       <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -515,8 +535,11 @@
       <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -526,8 +549,9 @@
       <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -537,8 +561,11 @@
       <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -546,60 +573,73 @@
         <v>0.5</v>
       </c>
       <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>